<commit_message>
VL48 - Quantity Facade testid ja klassid
</commit_message>
<xml_diff>
--- a/AJALOGI/PROGE_Time recording log.xlsx
+++ b/AJALOGI/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\VL\AJALOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA336F9E-BE9A-47C7-A518-993E10613532}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B314C783-FC6B-4121-852A-71C74FE5A127}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1440" windowWidth="21600" windowHeight="11325" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="196">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -622,6 +622,15 @@
   </si>
   <si>
     <t>Uus projekt korda</t>
+  </si>
+  <si>
+    <t>VL48</t>
+  </si>
+  <si>
+    <t>VL48 jätk</t>
+  </si>
+  <si>
+    <t>Quantity façade testid ja klassid</t>
   </si>
 </sst>
 </file>
@@ -7306,10 +7315,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -7679,7 +7689,9 @@
       <c r="H15" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1">
@@ -7768,14 +7780,22 @@
         <v>12</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="7">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.91736111111111107</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
       <c r="F19" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>193</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
@@ -7786,16 +7806,28 @@
         <v>13</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="7">
+        <v>0.94305555555555554</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
       <c r="F20" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+        <v>34.000000000000043</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1">
@@ -7862,7 +7894,7 @@
       <c r="E24" s="97"/>
       <c r="F24" s="31">
         <f>SUM(F7:F23)</f>
-        <v>385.99999999999994</v>
+        <v>510</v>
       </c>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>

</xml_diff>

<commit_message>
VL50-Infra FilteredRepository testid VL51 (47min)-Infra PaginatedRepository testid
</commit_message>
<xml_diff>
--- a/AJALOGI/PROGE_Time recording log.xlsx
+++ b/AJALOGI/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\VL\AJALOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B4AEB7-AC41-4635-816B-156936738E5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F2C4CA-2C29-4551-9538-A1A4F50DAB92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12855" yWindow="1755" windowWidth="21600" windowHeight="11325" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10485" yWindow="3285" windowWidth="21600" windowHeight="11325" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="205">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -643,6 +643,21 @@
   </si>
   <si>
     <t>Infra FilteredRepository testid</t>
+  </si>
+  <si>
+    <t>VL51</t>
+  </si>
+  <si>
+    <t>VL52</t>
+  </si>
+  <si>
+    <t>Infra PaginatedRepository testid</t>
+  </si>
+  <si>
+    <t> Infra MeasuresRepository testid</t>
+  </si>
+  <si>
+    <t>VL51 jätk</t>
   </si>
 </sst>
 </file>
@@ -652,7 +667,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,16 +694,43 @@
       <name val="Calibri "/>
       <charset val="186"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1002,11 +1044,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1256,8 +1314,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7328,16 +7438,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
@@ -7406,575 +7516,617 @@
       <c r="I5" s="108"/>
       <c r="J5" s="109"/>
     </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="32.25" thickBot="1">
+      <c r="A6" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="126" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="14">
+    <row r="7" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A7" s="127">
         <v>1</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="128">
         <v>43916</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="129">
         <v>0.48472222222222222</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="129">
         <v>0.50763888888888886</v>
       </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
+      <c r="E7" s="130">
+        <v>0</v>
+      </c>
+      <c r="F7" s="131">
         <f>(D7-C7)*1440</f>
         <v>32.999999999999964</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="130" t="s">
         <v>177</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="132"/>
       <c r="N7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A8" s="14">
+    <row r="8" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A8" s="127">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7">
+      <c r="B8" s="133"/>
+      <c r="C8" s="134">
         <v>0.94305555555555554</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="134">
         <v>0.96875</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
-        <f t="shared" ref="F8:F26" si="0">(D8-C8)*1440</f>
+      <c r="E8" s="135">
+        <v>0</v>
+      </c>
+      <c r="F8" s="131">
+        <f t="shared" ref="F8:F27" si="0">(D8-C8)*1440</f>
         <v>37.000000000000028</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="135" t="s">
         <v>179</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="J8" s="136"/>
       <c r="N8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A9" s="14">
-        <f t="shared" ref="A9:A26" si="1">A8+1</f>
+    <row r="9" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A9" s="127">
+        <f t="shared" ref="A9:A21" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="133">
         <v>43917</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="134">
         <v>0.40416666666666662</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="134">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
+      <c r="E9" s="135">
+        <v>0</v>
+      </c>
+      <c r="F9" s="131">
         <f t="shared" si="0"/>
         <v>18.000000000000096</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="135" t="s">
         <v>181</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="135" t="s">
         <v>182</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A10" s="14">
+      <c r="J9" s="136"/>
+    </row>
+    <row r="10" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A10" s="127">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7">
+      <c r="B10" s="133"/>
+      <c r="C10" s="134">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="134">
         <v>0.46180555555555558</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
+      <c r="E10" s="135">
+        <v>0</v>
+      </c>
+      <c r="F10" s="131">
         <f t="shared" si="0"/>
         <v>25.000000000000071</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="135" t="s">
         <v>183</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A11" s="14">
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="136"/>
+    </row>
+    <row r="11" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A11" s="127">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="133">
         <v>43919</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="134">
         <v>0.90972222222222221</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="134">
         <v>0.9291666666666667</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30">
+      <c r="E11" s="135">
+        <v>0</v>
+      </c>
+      <c r="F11" s="131">
         <f t="shared" si="0"/>
         <v>28.00000000000006</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="135" t="s">
         <v>184</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A12" s="14">
+      <c r="I11" s="135"/>
+      <c r="J11" s="136"/>
+    </row>
+    <row r="12" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A12" s="127">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7">
+      <c r="B12" s="133"/>
+      <c r="C12" s="134">
         <v>0.97013888888888899</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="134">
         <v>0.98958333333333337</v>
       </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30">
+      <c r="E12" s="135">
+        <v>0</v>
+      </c>
+      <c r="F12" s="131">
         <f t="shared" si="0"/>
         <v>27.999999999999901</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="135" t="s">
         <v>184</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="14">
+      <c r="I12" s="135"/>
+      <c r="J12" s="136"/>
+    </row>
+    <row r="13" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A13" s="127">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="133">
         <v>43920</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="134">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="134">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="30">
+      <c r="E13" s="135">
+        <v>0</v>
+      </c>
+      <c r="F13" s="131">
         <f t="shared" si="0"/>
         <v>35.000000000000036</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="135" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="14">
+      <c r="J13" s="136"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A14" s="127">
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7">
+      <c r="B14" s="133"/>
+      <c r="C14" s="134">
         <v>0.8666666666666667</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="134">
         <v>0.88888888888888884</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30">
+      <c r="E14" s="135">
+        <v>0</v>
+      </c>
+      <c r="F14" s="131">
         <f t="shared" si="0"/>
         <v>31.999999999999886</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="135" t="s">
         <v>188</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A15" s="14">
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
+      <c r="J14" s="136"/>
+    </row>
+    <row r="15" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A15" s="127">
         <v>9</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="133">
         <v>43921</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="134">
         <v>0.44375000000000003</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="134">
         <v>0.4694444444444445</v>
       </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="30">
+      <c r="E15" s="135">
+        <v>0</v>
+      </c>
+      <c r="F15" s="131">
         <f t="shared" si="0"/>
         <v>37.000000000000028</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="135" t="s">
         <v>186</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="135" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A16" s="14">
+      <c r="J15" s="136"/>
+    </row>
+    <row r="16" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A16" s="127">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7">
+      <c r="B16" s="133"/>
+      <c r="C16" s="134">
         <v>0.4694444444444445</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="134">
         <v>0.48888888888888887</v>
       </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="30">
+      <c r="E16" s="135">
+        <v>0</v>
+      </c>
+      <c r="F16" s="131">
         <f t="shared" si="0"/>
         <v>27.999999999999901</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="135" t="s">
         <v>189</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A17" s="14">
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="136"/>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A17" s="127">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7">
+      <c r="B17" s="133"/>
+      <c r="C17" s="134">
         <v>0.57777777777777783</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="134">
         <v>0.62916666666666665</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="30">
+      <c r="E17" s="135">
+        <v>0</v>
+      </c>
+      <c r="F17" s="131">
         <f t="shared" si="0"/>
         <v>73.999999999999901</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="135" t="s">
         <v>191</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A18" s="14">
+      <c r="I17" s="135"/>
+      <c r="J17" s="136"/>
+    </row>
+    <row r="18" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A18" s="127">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7">
+      <c r="B18" s="133"/>
+      <c r="C18" s="134">
         <v>0.80555555555555547</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="134">
         <v>0.81319444444444444</v>
       </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="30">
+      <c r="E18" s="135">
+        <v>0</v>
+      </c>
+      <c r="F18" s="131">
         <f t="shared" si="0"/>
         <v>11.000000000000121</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="135" t="s">
         <v>192</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A19" s="14">
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="136"/>
+    </row>
+    <row r="19" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A19" s="127">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7">
+      <c r="B19" s="133"/>
+      <c r="C19" s="134">
         <v>0.85486111111111107</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="134">
         <v>0.91736111111111107</v>
       </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="30">
+      <c r="E19" s="135">
+        <v>0</v>
+      </c>
+      <c r="F19" s="131">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A20" s="14">
+      <c r="H19" s="135"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="136"/>
+    </row>
+    <row r="20" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A20" s="127">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7">
+      <c r="B20" s="133"/>
+      <c r="C20" s="134">
         <v>0.94305555555555554</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="134">
         <v>0.96666666666666667</v>
       </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="30">
+      <c r="E20" s="135">
+        <v>0</v>
+      </c>
+      <c r="F20" s="131">
         <f t="shared" si="0"/>
         <v>34.000000000000043</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="135" t="s">
         <v>194</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="135" t="s">
         <v>195</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A21" s="14">
+      <c r="J20" s="136"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A21" s="127">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="133">
         <v>43922</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="134">
         <v>0.37777777777777777</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="134">
         <v>0.4201388888888889</v>
       </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="30">
+      <c r="E21" s="135">
+        <v>0</v>
+      </c>
+      <c r="F21" s="131">
         <f t="shared" si="0"/>
         <v>61.000000000000021</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="135" t="s">
         <v>197</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A22" s="14">
+      <c r="J21" s="136"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A22" s="127">
         <v>16</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="5" t="s">
+      <c r="B22" s="133"/>
+      <c r="C22" s="134">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D22" s="134">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E22" s="135">
+        <v>0</v>
+      </c>
+      <c r="F22" s="131">
+        <f t="shared" si="0"/>
+        <v>70.000000000000071</v>
+      </c>
+      <c r="G22" s="135" t="s">
         <v>198</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="135" t="s">
         <v>199</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="14">
+      <c r="I22" s="135" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="136"/>
+    </row>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A23" s="127">
         <v>17</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A24" s="14">
+      <c r="B23" s="133"/>
+      <c r="C23" s="134">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D23" s="134">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="E23" s="135">
+        <v>0</v>
+      </c>
+      <c r="F23" s="131">
+        <f t="shared" si="0"/>
+        <v>43.999999999999922</v>
+      </c>
+      <c r="G23" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="H23" s="147" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="135"/>
+      <c r="J23" s="136"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A24" s="127"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="135" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="147"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="136"/>
+    </row>
+    <row r="25" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A25" s="127">
         <v>18</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A25" s="14">
+      <c r="B25" s="133"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="131"/>
+      <c r="G25" s="135" t="s">
+        <v>201</v>
+      </c>
+      <c r="H25" s="147" t="s">
+        <v>203</v>
+      </c>
+      <c r="I25" s="135"/>
+      <c r="J25" s="136"/>
+    </row>
+    <row r="26" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A26" s="127">
         <v>19</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A26" s="14">
+      <c r="B26" s="133"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="131">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="135"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="135"/>
+      <c r="J26" s="136"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A27" s="127">
         <v>20</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A27" s="95" t="s">
+      <c r="B27" s="137"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="131">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="139"/>
+      <c r="H27" s="139"/>
+      <c r="I27" s="139"/>
+      <c r="J27" s="140"/>
+    </row>
+    <row r="28" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A28" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="31">
-        <f>SUM(F7:F26)</f>
-        <v>571</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="24"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="143"/>
+      <c r="F28" s="144">
+        <f>SUM(F7:F27)</f>
+        <v>685</v>
+      </c>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
@@ -7983,6 +8135,6 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
VL51 jätk; paginatedRepositoryTests korda
</commit_message>
<xml_diff>
--- a/AJALOGI/PROGE_Time recording log.xlsx
+++ b/AJALOGI/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\VL\AJALOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F2C4CA-2C29-4551-9538-A1A4F50DAB92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C68813-E054-4252-96E5-72628F943FDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10485" yWindow="3285" windowWidth="21600" windowHeight="11325" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="206">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>VL51 jätk</t>
+  </si>
+  <si>
+    <t>+vigade parandused</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1230,6 +1233,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1314,38 +1353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1355,16 +1362,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1687,85 +1691,85 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105">
+      <c r="G4" s="127">
         <v>43863</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1791,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -1854,7 +1858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -1882,7 +1886,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1912,7 +1916,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1940,7 +1944,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1968,7 +1972,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1996,7 +2000,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2024,7 +2028,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2052,7 +2056,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2084,7 +2088,7 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2112,7 +2116,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2142,7 +2146,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2172,7 +2176,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2200,7 +2204,7 @@
       </c>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2228,7 +2232,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2246,14 +2250,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="95" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -2287,83 +2291,83 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -2432,7 +2436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -2450,7 +2454,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2468,7 +2472,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2486,7 +2490,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2504,7 +2508,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2522,7 +2526,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2540,7 +2544,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2558,7 +2562,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2576,7 +2580,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2594,7 +2598,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2612,7 +2616,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2630,7 +2634,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2648,7 +2652,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2666,7 +2670,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2684,14 +2688,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="95" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>0</v>
@@ -2725,85 +2729,85 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105">
+      <c r="G4" s="127">
         <v>43871</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -2896,7 +2900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A21" si="1">A8+1</f>
         <v>3</v>
@@ -2924,7 +2928,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2956,7 +2960,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2986,7 +2990,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3016,7 +3020,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3046,7 +3050,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3076,7 +3080,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3106,7 +3110,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3132,7 +3136,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3158,7 +3162,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3186,7 +3190,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3214,7 +3218,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3242,7 +3246,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3268,7 +3272,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27">
@@ -3291,7 +3295,7 @@
       <c r="I22" s="28"/>
       <c r="J22" s="29"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14"/>
       <c r="B23" s="26"/>
       <c r="C23" s="27">
@@ -3314,7 +3318,7 @@
       <c r="I23" s="28"/>
       <c r="J23" s="29"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27">
@@ -3337,7 +3341,7 @@
       <c r="I24" s="28"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14"/>
       <c r="B25" s="26">
         <v>43870</v>
@@ -3364,7 +3368,7 @@
       <c r="I25" s="28"/>
       <c r="J25" s="29"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <f>A21+1</f>
         <v>16</v>
@@ -3390,14 +3394,14 @@
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A27" s="95" t="s">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="A27" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="119"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -3431,83 +3435,83 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -3563,7 +3567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -3596,7 +3600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -3624,7 +3628,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3652,7 +3656,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3680,7 +3684,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3706,7 +3710,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3736,7 +3740,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3762,7 +3766,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3790,7 +3794,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3818,7 +3822,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3846,7 +3850,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3872,7 +3876,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3890,7 +3894,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3908,7 +3912,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3926,7 +3930,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -3944,14 +3948,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="95" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -3985,22 +3989,22 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="72.140625" style="39" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="72.109375" style="39" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
       <c r="A2" s="43" t="s">
         <v>0</v>
@@ -4027,7 +4031,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+    <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="49" t="s">
         <v>1</v>
       </c>
@@ -4045,7 +4049,7 @@
       <c r="I4" s="52"/>
       <c r="J4" s="53"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+    <row r="5" spans="1:14" ht="15" thickBot="1">
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -4057,7 +4061,7 @@
       <c r="I5" s="55"/>
       <c r="J5" s="56"/>
     </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
       <c r="A6" s="57" t="s">
         <v>3</v>
       </c>
@@ -4087,7 +4091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -4117,7 +4121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -4148,7 +4152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -4176,7 +4180,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4204,7 +4208,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4236,7 +4240,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4262,7 +4266,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4294,7 +4298,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4320,7 +4324,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4350,7 +4354,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" s="39" customFormat="1" ht="60.75" thickBot="1">
+    <row r="16" spans="1:14" s="39" customFormat="1" ht="43.8" thickBot="1">
       <c r="A16" s="32">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4382,7 +4386,7 @@
       </c>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="1:10" ht="30.75" thickBot="1">
+    <row r="17" spans="1:10" ht="29.4" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4412,7 +4416,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4440,7 +4444,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4458,7 +4462,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4476,7 +4480,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4494,7 +4498,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -4512,7 +4516,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="40" t="s">
         <v>21</v>
       </c>
@@ -4544,83 +4548,83 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="92.85546875" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="92.88671875" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4646,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -4676,7 +4680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -4711,7 +4715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A20" si="1">A8+1</f>
         <v>3</v>
@@ -4739,7 +4743,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4769,7 +4773,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4799,7 +4803,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4827,7 +4831,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4857,7 +4861,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4885,7 +4889,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4913,7 +4917,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4941,7 +4945,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4969,7 +4973,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4999,7 +5003,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -5029,7 +5033,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5059,7 +5063,7 @@
       </c>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <v>15</v>
       </c>
@@ -5088,7 +5092,7 @@
       </c>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -5115,7 +5119,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -5144,7 +5148,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14">
         <v>18</v>
       </c>
@@ -5161,7 +5165,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -5178,7 +5182,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <v>20</v>
       </c>
@@ -5195,7 +5199,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
       <c r="A27" s="14">
         <v>21</v>
       </c>
@@ -5212,14 +5216,14 @@
       <c r="I27" s="21"/>
       <c r="J27" s="22"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A28" s="112" t="s">
+    <row r="28" spans="1:10" ht="15" thickBot="1">
+      <c r="A28" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="114"/>
+      <c r="B28" s="135"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
         <v>1058.0000000000002</v>
@@ -5253,83 +5257,83 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5355,7 +5359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -5389,7 +5393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <v>2</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <v>3</v>
       </c>
@@ -5448,7 +5452,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <v>4</v>
       </c>
@@ -5476,7 +5480,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <v>5</v>
       </c>
@@ -5505,7 +5509,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <v>6</v>
       </c>
@@ -5536,7 +5540,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <v>7</v>
       </c>
@@ -5563,7 +5567,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <v>8</v>
       </c>
@@ -5588,7 +5592,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <v>9</v>
       </c>
@@ -5615,7 +5619,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <v>10</v>
       </c>
@@ -5640,7 +5644,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <v>11</v>
       </c>
@@ -5669,7 +5673,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <v>12</v>
       </c>
@@ -5698,7 +5702,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <v>13</v>
       </c>
@@ -5723,7 +5727,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <v>14</v>
       </c>
@@ -5748,7 +5752,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <v>15</v>
       </c>
@@ -5777,7 +5781,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -5806,7 +5810,7 @@
       </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -5837,7 +5841,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14">
         <v>18</v>
       </c>
@@ -5866,7 +5870,7 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -5883,7 +5887,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <v>20</v>
       </c>
@@ -5900,14 +5904,14 @@
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A27" s="95" t="s">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="A27" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="119"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>702.99999999999989</v>
@@ -5941,85 +5945,85 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="69" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="70" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="71" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="71" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="69" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="69" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="70" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="71" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="71" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="69" customWidth="1"/>
     <col min="6" max="6" width="11" style="72" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" style="69" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" style="69" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="69" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="69" customWidth="1"/>
-    <col min="11" max="13" width="8.7109375" style="69"/>
-    <col min="14" max="14" width="26.7109375" style="69" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="69"/>
+    <col min="7" max="7" width="55.6640625" style="69" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" style="69" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="69" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="69" customWidth="1"/>
+    <col min="11" max="13" width="8.6640625" style="69"/>
+    <col min="14" max="14" width="26.6640625" style="69" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="115" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="117"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="118"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="120"/>
-    </row>
-    <row r="6" spans="1:14" s="73" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="139"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="140"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="142"/>
+    </row>
+    <row r="6" spans="1:14" s="73" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6045,7 +6049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="74">
         <v>1</v>
       </c>
@@ -6077,7 +6081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="74">
         <f>A7+1</f>
         <v>2</v>
@@ -6108,7 +6112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="74">
         <f>A8+1</f>
         <v>3</v>
@@ -6136,7 +6140,7 @@
       </c>
       <c r="J9" s="83"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="74">
         <v>4</v>
       </c>
@@ -6165,7 +6169,7 @@
       <c r="I10" s="82"/>
       <c r="J10" s="83"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="74">
         <f>A10+1</f>
         <v>5</v>
@@ -6195,7 +6199,7 @@
       </c>
       <c r="J11" s="83"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="74">
         <f>A11+1</f>
         <v>6</v>
@@ -6223,7 +6227,7 @@
       <c r="I12" s="82"/>
       <c r="J12" s="83"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="74">
         <v>7</v>
       </c>
@@ -6250,7 +6254,7 @@
       </c>
       <c r="J13" s="83"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="74">
         <f>A13+1</f>
         <v>8</v>
@@ -6278,7 +6282,7 @@
       <c r="I14" s="82"/>
       <c r="J14" s="83"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="74">
         <f>A14+1</f>
         <v>9</v>
@@ -6306,7 +6310,7 @@
       </c>
       <c r="J15" s="83"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="74">
         <v>10</v>
       </c>
@@ -6331,7 +6335,7 @@
       <c r="I16" s="82"/>
       <c r="J16" s="83"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="74">
         <f>A16+1</f>
         <v>11</v>
@@ -6361,7 +6365,7 @@
       <c r="I17" s="82"/>
       <c r="J17" s="83"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="74">
         <f>A17+1</f>
         <v>12</v>
@@ -6387,7 +6391,7 @@
       <c r="I18" s="82"/>
       <c r="J18" s="83"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="74">
         <v>13</v>
       </c>
@@ -6412,7 +6416,7 @@
       <c r="I19" s="82"/>
       <c r="J19" s="83"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="74">
         <f>A19+1</f>
         <v>14</v>
@@ -6438,7 +6442,7 @@
       <c r="I20" s="82"/>
       <c r="J20" s="83"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="74">
         <f>A20+1</f>
         <v>15</v>
@@ -6466,7 +6470,7 @@
       <c r="I21" s="82"/>
       <c r="J21" s="83"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="74">
         <v>16</v>
       </c>
@@ -6495,7 +6499,7 @@
       </c>
       <c r="J22" s="83"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="74">
         <f>A22+1</f>
         <v>17</v>
@@ -6521,7 +6525,7 @@
       <c r="I23" s="82"/>
       <c r="J23" s="83"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="74">
         <f>A23+1</f>
         <v>18</v>
@@ -6549,7 +6553,7 @@
       </c>
       <c r="J24" s="83"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="74">
         <v>19</v>
       </c>
@@ -6580,7 +6584,7 @@
       </c>
       <c r="J25" s="83"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="74">
         <f>A25+1</f>
         <v>20</v>
@@ -6612,7 +6616,7 @@
       </c>
       <c r="J26" s="83"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
       <c r="A27" s="74">
         <f>A26+1</f>
         <v>21</v>
@@ -6642,7 +6646,7 @@
       </c>
       <c r="J27" s="83"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1">
+    <row r="28" spans="1:10" ht="15" thickBot="1">
       <c r="A28" s="74">
         <v>22</v>
       </c>
@@ -6659,7 +6663,7 @@
       <c r="I28" s="82"/>
       <c r="J28" s="83"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1">
+    <row r="29" spans="1:10" ht="15" thickBot="1">
       <c r="A29" s="74">
         <f>A28+1</f>
         <v>23</v>
@@ -6677,7 +6681,7 @@
       <c r="I29" s="82"/>
       <c r="J29" s="83"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1">
+    <row r="30" spans="1:10" ht="15" thickBot="1">
       <c r="A30" s="74">
         <f>A29+1</f>
         <v>24</v>
@@ -6695,7 +6699,7 @@
       <c r="I30" s="82"/>
       <c r="J30" s="83"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1">
+    <row r="31" spans="1:10" ht="15" thickBot="1">
       <c r="A31" s="74">
         <v>25</v>
       </c>
@@ -6712,7 +6716,7 @@
       <c r="I31" s="82"/>
       <c r="J31" s="83"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1">
+    <row r="32" spans="1:10" ht="15" thickBot="1">
       <c r="A32" s="74">
         <f>A31+1</f>
         <v>26</v>
@@ -6730,14 +6734,14 @@
       <c r="I32" s="87"/>
       <c r="J32" s="88"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A33" s="95" t="s">
+    <row r="33" spans="1:10" ht="15" thickBot="1">
+      <c r="A33" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="119"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
         <v>1039.0000000000007</v>
@@ -6771,83 +6775,83 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6873,7 +6877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -6907,7 +6911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <v>2</v>
       </c>
@@ -6939,7 +6943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <v>3</v>
       </c>
@@ -6964,7 +6968,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <v>4</v>
       </c>
@@ -6991,7 +6995,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <v>5</v>
       </c>
@@ -7016,7 +7020,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <v>6</v>
       </c>
@@ -7045,7 +7049,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <v>7</v>
       </c>
@@ -7070,7 +7074,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <v>8</v>
       </c>
@@ -7097,7 +7101,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <v>9</v>
       </c>
@@ -7124,7 +7128,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <v>10</v>
       </c>
@@ -7153,7 +7157,7 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <v>11</v>
       </c>
@@ -7182,7 +7186,7 @@
       </c>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <v>12</v>
       </c>
@@ -7209,7 +7213,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <v>13</v>
       </c>
@@ -7234,7 +7238,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <v>14</v>
       </c>
@@ -7261,7 +7265,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <v>15</v>
       </c>
@@ -7290,7 +7294,7 @@
       </c>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -7317,7 +7321,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -7344,7 +7348,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14">
         <v>18</v>
       </c>
@@ -7369,7 +7373,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -7386,7 +7390,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <v>20</v>
       </c>
@@ -7403,14 +7407,14 @@
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A27" s="95" t="s">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="A27" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="119"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>838.99999999999932</v>
@@ -7440,689 +7444,702 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="110" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="32.25" thickBot="1">
-      <c r="A6" s="121" t="s">
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="31.8" thickBot="1">
+      <c r="A6" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="122"/>
-      <c r="C6" s="123" t="s">
+      <c r="B6" s="147"/>
+      <c r="C6" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="123" t="s">
+      <c r="D6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="124" t="s">
+      <c r="E6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="124" t="s">
+      <c r="G6" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="124" t="s">
+      <c r="H6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="124" t="s">
+      <c r="I6" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="126" t="s">
+      <c r="J6" s="96" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A7" s="127">
+    <row r="7" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A7" s="97">
         <v>1</v>
       </c>
-      <c r="B7" s="128">
+      <c r="B7" s="98">
         <v>43916</v>
       </c>
-      <c r="C7" s="129">
+      <c r="C7" s="99">
         <v>0.48472222222222222</v>
       </c>
-      <c r="D7" s="129">
+      <c r="D7" s="99">
         <v>0.50763888888888886</v>
       </c>
-      <c r="E7" s="130">
-        <v>0</v>
-      </c>
-      <c r="F7" s="131">
+      <c r="E7" s="100">
+        <v>0</v>
+      </c>
+      <c r="F7" s="101">
         <f>(D7-C7)*1440</f>
         <v>32.999999999999964</v>
       </c>
-      <c r="G7" s="130" t="s">
+      <c r="G7" s="100" t="s">
         <v>177</v>
       </c>
-      <c r="H7" s="130" t="s">
+      <c r="H7" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="I7" s="130" t="s">
+      <c r="I7" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="132"/>
+      <c r="J7" s="102"/>
       <c r="N7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A8" s="127">
+    <row r="8" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A8" s="97">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="133"/>
-      <c r="C8" s="134">
+      <c r="B8" s="103"/>
+      <c r="C8" s="104">
         <v>0.94305555555555554</v>
       </c>
-      <c r="D8" s="134">
+      <c r="D8" s="104">
         <v>0.96875</v>
       </c>
-      <c r="E8" s="135">
-        <v>0</v>
-      </c>
-      <c r="F8" s="131">
+      <c r="E8" s="105">
+        <v>0</v>
+      </c>
+      <c r="F8" s="101">
         <f t="shared" ref="F8:F27" si="0">(D8-C8)*1440</f>
         <v>37.000000000000028</v>
       </c>
-      <c r="G8" s="135" t="s">
+      <c r="G8" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="H8" s="135" t="s">
+      <c r="H8" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="I8" s="135" t="s">
+      <c r="I8" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="136"/>
+      <c r="J8" s="106"/>
       <c r="N8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A9" s="127">
+    <row r="9" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A9" s="97">
         <f t="shared" ref="A9:A21" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="133">
+      <c r="B9" s="103">
         <v>43917</v>
       </c>
-      <c r="C9" s="134">
+      <c r="C9" s="104">
         <v>0.40416666666666662</v>
       </c>
-      <c r="D9" s="134">
+      <c r="D9" s="104">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E9" s="135">
-        <v>0</v>
-      </c>
-      <c r="F9" s="131">
+      <c r="E9" s="105">
+        <v>0</v>
+      </c>
+      <c r="F9" s="101">
         <f t="shared" si="0"/>
         <v>18.000000000000096</v>
       </c>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="105" t="s">
         <v>181</v>
       </c>
-      <c r="H9" s="135" t="s">
+      <c r="H9" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="I9" s="135" t="s">
+      <c r="I9" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="136"/>
-    </row>
-    <row r="10" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A10" s="127">
+      <c r="J9" s="106"/>
+    </row>
+    <row r="10" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A10" s="97">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="133"/>
-      <c r="C10" s="134">
+      <c r="B10" s="103"/>
+      <c r="C10" s="104">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D10" s="134">
+      <c r="D10" s="104">
         <v>0.46180555555555558</v>
       </c>
-      <c r="E10" s="135">
-        <v>0</v>
-      </c>
-      <c r="F10" s="131">
+      <c r="E10" s="105">
+        <v>0</v>
+      </c>
+      <c r="F10" s="101">
         <f t="shared" si="0"/>
         <v>25.000000000000071</v>
       </c>
-      <c r="G10" s="135" t="s">
+      <c r="G10" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="136"/>
-    </row>
-    <row r="11" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A11" s="127">
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="106"/>
+    </row>
+    <row r="11" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A11" s="97">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="133">
+      <c r="B11" s="103">
         <v>43919</v>
       </c>
-      <c r="C11" s="134">
+      <c r="C11" s="104">
         <v>0.90972222222222221</v>
       </c>
-      <c r="D11" s="134">
+      <c r="D11" s="104">
         <v>0.9291666666666667</v>
       </c>
-      <c r="E11" s="135">
-        <v>0</v>
-      </c>
-      <c r="F11" s="131">
+      <c r="E11" s="105">
+        <v>0</v>
+      </c>
+      <c r="F11" s="101">
         <f t="shared" si="0"/>
         <v>28.00000000000006</v>
       </c>
-      <c r="G11" s="135" t="s">
+      <c r="G11" s="105" t="s">
         <v>184</v>
       </c>
-      <c r="H11" s="135" t="s">
+      <c r="H11" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="135"/>
-      <c r="J11" s="136"/>
-    </row>
-    <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="127">
+      <c r="I11" s="105"/>
+      <c r="J11" s="106"/>
+    </row>
+    <row r="12" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A12" s="97">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="134">
+      <c r="B12" s="103"/>
+      <c r="C12" s="104">
         <v>0.97013888888888899</v>
       </c>
-      <c r="D12" s="134">
+      <c r="D12" s="104">
         <v>0.98958333333333337</v>
       </c>
-      <c r="E12" s="135">
-        <v>0</v>
-      </c>
-      <c r="F12" s="131">
+      <c r="E12" s="105">
+        <v>0</v>
+      </c>
+      <c r="F12" s="101">
         <f t="shared" si="0"/>
         <v>27.999999999999901</v>
       </c>
-      <c r="G12" s="135" t="s">
+      <c r="G12" s="105" t="s">
         <v>184</v>
       </c>
-      <c r="H12" s="135" t="s">
+      <c r="H12" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="I12" s="135"/>
-      <c r="J12" s="136"/>
-    </row>
-    <row r="13" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A13" s="127">
+      <c r="I12" s="105"/>
+      <c r="J12" s="106"/>
+    </row>
+    <row r="13" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A13" s="97">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="133">
+      <c r="B13" s="103">
         <v>43920</v>
       </c>
-      <c r="C13" s="134">
+      <c r="C13" s="104">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D13" s="134">
+      <c r="D13" s="104">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E13" s="135">
-        <v>0</v>
-      </c>
-      <c r="F13" s="131">
+      <c r="E13" s="105">
+        <v>0</v>
+      </c>
+      <c r="F13" s="101">
         <f t="shared" si="0"/>
         <v>35.000000000000036</v>
       </c>
-      <c r="G13" s="135" t="s">
+      <c r="G13" s="105" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="135" t="s">
+      <c r="H13" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="I13" s="135" t="s">
+      <c r="I13" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="136"/>
-    </row>
-    <row r="14" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A14" s="127">
+      <c r="J13" s="106"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A14" s="97">
         <v>8</v>
       </c>
-      <c r="B14" s="133"/>
-      <c r="C14" s="134">
+      <c r="B14" s="103"/>
+      <c r="C14" s="104">
         <v>0.8666666666666667</v>
       </c>
-      <c r="D14" s="134">
+      <c r="D14" s="104">
         <v>0.88888888888888884</v>
       </c>
-      <c r="E14" s="135">
-        <v>0</v>
-      </c>
-      <c r="F14" s="131">
+      <c r="E14" s="105">
+        <v>0</v>
+      </c>
+      <c r="F14" s="101">
         <f t="shared" si="0"/>
         <v>31.999999999999886</v>
       </c>
-      <c r="G14" s="135" t="s">
+      <c r="G14" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="H14" s="135"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="136"/>
-    </row>
-    <row r="15" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A15" s="127">
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="106"/>
+    </row>
+    <row r="15" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A15" s="97">
         <v>9</v>
       </c>
-      <c r="B15" s="133">
+      <c r="B15" s="103">
         <v>43921</v>
       </c>
-      <c r="C15" s="134">
+      <c r="C15" s="104">
         <v>0.44375000000000003</v>
       </c>
-      <c r="D15" s="134">
+      <c r="D15" s="104">
         <v>0.4694444444444445</v>
       </c>
-      <c r="E15" s="135">
-        <v>0</v>
-      </c>
-      <c r="F15" s="131">
+      <c r="E15" s="105">
+        <v>0</v>
+      </c>
+      <c r="F15" s="101">
         <f t="shared" si="0"/>
         <v>37.000000000000028</v>
       </c>
-      <c r="G15" s="135" t="s">
+      <c r="G15" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="H15" s="135" t="s">
+      <c r="H15" s="105" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="135" t="s">
+      <c r="I15" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="136"/>
-    </row>
-    <row r="16" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A16" s="127">
+      <c r="J15" s="106"/>
+    </row>
+    <row r="16" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A16" s="97">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="133"/>
-      <c r="C16" s="134">
+      <c r="B16" s="103"/>
+      <c r="C16" s="104">
         <v>0.4694444444444445</v>
       </c>
-      <c r="D16" s="134">
+      <c r="D16" s="104">
         <v>0.48888888888888887</v>
       </c>
-      <c r="E16" s="135">
-        <v>0</v>
-      </c>
-      <c r="F16" s="131">
+      <c r="E16" s="105">
+        <v>0</v>
+      </c>
+      <c r="F16" s="101">
         <f t="shared" si="0"/>
         <v>27.999999999999901</v>
       </c>
-      <c r="G16" s="135" t="s">
+      <c r="G16" s="105" t="s">
         <v>189</v>
       </c>
-      <c r="H16" s="135"/>
-      <c r="I16" s="135"/>
-      <c r="J16" s="136"/>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A17" s="127">
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="106"/>
+    </row>
+    <row r="17" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A17" s="97">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="134">
+      <c r="B17" s="103"/>
+      <c r="C17" s="104">
         <v>0.57777777777777783</v>
       </c>
-      <c r="D17" s="134">
+      <c r="D17" s="104">
         <v>0.62916666666666665</v>
       </c>
-      <c r="E17" s="135">
-        <v>0</v>
-      </c>
-      <c r="F17" s="131">
+      <c r="E17" s="105">
+        <v>0</v>
+      </c>
+      <c r="F17" s="101">
         <f t="shared" si="0"/>
         <v>73.999999999999901</v>
       </c>
-      <c r="G17" s="135" t="s">
+      <c r="G17" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="H17" s="135" t="s">
+      <c r="H17" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="I17" s="135"/>
-      <c r="J17" s="136"/>
-    </row>
-    <row r="18" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A18" s="127">
+      <c r="I17" s="105"/>
+      <c r="J17" s="106"/>
+    </row>
+    <row r="18" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A18" s="97">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="133"/>
-      <c r="C18" s="134">
+      <c r="B18" s="103"/>
+      <c r="C18" s="104">
         <v>0.80555555555555547</v>
       </c>
-      <c r="D18" s="134">
+      <c r="D18" s="104">
         <v>0.81319444444444444</v>
       </c>
-      <c r="E18" s="135">
-        <v>0</v>
-      </c>
-      <c r="F18" s="131">
+      <c r="E18" s="105">
+        <v>0</v>
+      </c>
+      <c r="F18" s="101">
         <f t="shared" si="0"/>
         <v>11.000000000000121</v>
       </c>
-      <c r="G18" s="135" t="s">
+      <c r="G18" s="105" t="s">
         <v>192</v>
       </c>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="136"/>
-    </row>
-    <row r="19" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A19" s="127">
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="106"/>
+    </row>
+    <row r="19" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A19" s="97">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B19" s="133"/>
-      <c r="C19" s="134">
+      <c r="B19" s="103"/>
+      <c r="C19" s="104">
         <v>0.85486111111111107</v>
       </c>
-      <c r="D19" s="134">
+      <c r="D19" s="104">
         <v>0.91736111111111107</v>
       </c>
-      <c r="E19" s="135">
-        <v>0</v>
-      </c>
-      <c r="F19" s="131">
+      <c r="E19" s="105">
+        <v>0</v>
+      </c>
+      <c r="F19" s="101">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="136"/>
-    </row>
-    <row r="20" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A20" s="127">
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="106"/>
+    </row>
+    <row r="20" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A20" s="97">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B20" s="133"/>
-      <c r="C20" s="134">
+      <c r="B20" s="103"/>
+      <c r="C20" s="104">
         <v>0.94305555555555554</v>
       </c>
-      <c r="D20" s="134">
+      <c r="D20" s="104">
         <v>0.96666666666666667</v>
       </c>
-      <c r="E20" s="135">
-        <v>0</v>
-      </c>
-      <c r="F20" s="131">
+      <c r="E20" s="105">
+        <v>0</v>
+      </c>
+      <c r="F20" s="101">
         <f t="shared" si="0"/>
         <v>34.000000000000043</v>
       </c>
-      <c r="G20" s="135" t="s">
+      <c r="G20" s="105" t="s">
         <v>194</v>
       </c>
-      <c r="H20" s="135" t="s">
+      <c r="H20" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="I20" s="135" t="s">
+      <c r="I20" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="136"/>
-    </row>
-    <row r="21" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A21" s="127">
+      <c r="J20" s="106"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A21" s="97">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="133">
+      <c r="B21" s="103">
         <v>43922</v>
       </c>
-      <c r="C21" s="134">
+      <c r="C21" s="104">
         <v>0.37777777777777777</v>
       </c>
-      <c r="D21" s="134">
+      <c r="D21" s="104">
         <v>0.4201388888888889</v>
       </c>
-      <c r="E21" s="135">
-        <v>0</v>
-      </c>
-      <c r="F21" s="131">
+      <c r="E21" s="105">
+        <v>0</v>
+      </c>
+      <c r="F21" s="101">
         <f t="shared" si="0"/>
         <v>61.000000000000021</v>
       </c>
-      <c r="G21" s="135" t="s">
+      <c r="G21" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="H21" s="135" t="s">
+      <c r="H21" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="I21" s="135" t="s">
+      <c r="I21" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="136"/>
-    </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A22" s="127">
+      <c r="J21" s="106"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A22" s="97">
         <v>16</v>
       </c>
-      <c r="B22" s="133"/>
-      <c r="C22" s="134">
+      <c r="B22" s="103"/>
+      <c r="C22" s="104">
         <v>0.4236111111111111</v>
       </c>
-      <c r="D22" s="134">
+      <c r="D22" s="104">
         <v>0.47222222222222227</v>
       </c>
-      <c r="E22" s="135">
-        <v>0</v>
-      </c>
-      <c r="F22" s="131">
+      <c r="E22" s="105">
+        <v>0</v>
+      </c>
+      <c r="F22" s="101">
         <f t="shared" si="0"/>
         <v>70.000000000000071</v>
       </c>
-      <c r="G22" s="135" t="s">
+      <c r="G22" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="H22" s="135" t="s">
+      <c r="H22" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="I22" s="135" t="s">
+      <c r="I22" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="136"/>
+      <c r="J22" s="106"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A23" s="127">
+      <c r="A23" s="97">
         <v>17</v>
       </c>
-      <c r="B23" s="133"/>
-      <c r="C23" s="134">
+      <c r="B23" s="103"/>
+      <c r="C23" s="104">
         <v>0.47222222222222227</v>
       </c>
-      <c r="D23" s="134">
+      <c r="D23" s="104">
         <v>0.50277777777777777</v>
       </c>
-      <c r="E23" s="135">
-        <v>0</v>
-      </c>
-      <c r="F23" s="131">
+      <c r="E23" s="105">
+        <v>0</v>
+      </c>
+      <c r="F23" s="101">
         <f t="shared" si="0"/>
         <v>43.999999999999922</v>
       </c>
-      <c r="G23" s="135" t="s">
+      <c r="G23" s="105" t="s">
         <v>200</v>
       </c>
-      <c r="H23" s="147" t="s">
+      <c r="H23" s="114" t="s">
         <v>202</v>
       </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="136"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="106"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A24" s="127"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="135" t="s">
+      <c r="A24" s="97"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="104">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D24" s="104">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="E24" s="105">
+        <v>0</v>
+      </c>
+      <c r="F24" s="101">
+        <f t="shared" si="0"/>
+        <v>18.999999999999932</v>
+      </c>
+      <c r="G24" s="105" t="s">
         <v>204</v>
       </c>
-      <c r="H24" s="147"/>
-      <c r="I24" s="135"/>
-      <c r="J24" s="136"/>
-    </row>
-    <row r="25" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A25" s="127">
+      <c r="H24" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="I24" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="106"/>
+    </row>
+    <row r="25" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A25" s="97">
         <v>18</v>
       </c>
-      <c r="B25" s="133"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="135"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="135" t="s">
+      <c r="B25" s="103"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="H25" s="147" t="s">
+      <c r="H25" s="114" t="s">
         <v>203</v>
       </c>
-      <c r="I25" s="135"/>
-      <c r="J25" s="136"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A26" s="127">
+      <c r="I25" s="105"/>
+      <c r="J25" s="106"/>
+    </row>
+    <row r="26" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A26" s="97">
         <v>19</v>
       </c>
-      <c r="B26" s="133"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="131">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="135"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="136"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A27" s="127">
+      <c r="B26" s="103"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="101">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="106"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A27" s="97">
         <v>20</v>
       </c>
-      <c r="B27" s="137"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="131">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="139"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="140"/>
-    </row>
-    <row r="28" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A28" s="141" t="s">
+      <c r="B27" s="107"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="101">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="110"/>
+    </row>
+    <row r="28" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A28" s="143" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="143"/>
-      <c r="F28" s="144">
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="111">
         <f>SUM(F7:F27)</f>
-        <v>685</v>
-      </c>
-      <c r="G28" s="145"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="146"/>
+        <v>703.99999999999989</v>
+      </c>
+      <c r="G28" s="112"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
VL52 -  Infra MeasuresRepository testid
</commit_message>
<xml_diff>
--- a/AJALOGI/PROGE_Time recording log.xlsx
+++ b/AJALOGI/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\VL\AJALOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C68813-E054-4252-96E5-72628F943FDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1DAA48-F6B0-4310-9AB2-4A1E6B1A7AC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1269,6 +1269,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1368,7 +1369,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1708,68 +1708,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127">
+      <c r="G4" s="128">
         <v>43863</v>
       </c>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2251,13 +2251,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="119"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -2308,66 +2308,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2689,13 +2689,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="119"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>0</v>
@@ -2746,68 +2746,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127">
+      <c r="G4" s="128">
         <v>43871</v>
       </c>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3395,13 +3395,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -3452,66 +3452,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3949,13 +3949,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="119"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -4565,66 +4565,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5217,13 +5217,13 @@
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1">
-      <c r="A28" s="134" t="s">
+      <c r="A28" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="135"/>
-      <c r="C28" s="135"/>
-      <c r="D28" s="135"/>
-      <c r="E28" s="136"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="137"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
         <v>1058.0000000000002</v>
@@ -5274,66 +5274,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5905,13 +5905,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>702.99999999999989</v>
@@ -5964,66 +5964,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="137" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="140"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="140"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
-      <c r="H5" s="141"/>
-      <c r="I5" s="141"/>
-      <c r="J5" s="142"/>
+      <c r="A5" s="141"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="143"/>
     </row>
     <row r="6" spans="1:14" s="73" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6735,13 +6735,13 @@
       <c r="J32" s="88"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="119"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="119"/>
+      <c r="E33" s="120"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
         <v>1039.0000000000007</v>
@@ -6792,66 +6792,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -7408,13 +7408,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>838.99999999999932</v>
@@ -7444,8 +7444,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -7465,66 +7465,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="A2" s="120" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
+      <c r="A2" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="123"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="31.8" thickBot="1">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="147"/>
+      <c r="B6" s="148"/>
       <c r="C6" s="93" t="s">
         <v>4</v>
       </c>
@@ -8046,7 +8046,9 @@
       <c r="J23" s="106"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A24" s="97"/>
+      <c r="A24" s="97">
+        <v>18</v>
+      </c>
       <c r="B24" s="103"/>
       <c r="C24" s="104">
         <v>0.61458333333333337</v>
@@ -8064,7 +8066,7 @@
       <c r="G24" s="105" t="s">
         <v>204</v>
       </c>
-      <c r="H24" s="148" t="s">
+      <c r="H24" s="115" t="s">
         <v>205</v>
       </c>
       <c r="I24" s="105" t="s">
@@ -8074,13 +8076,22 @@
     </row>
     <row r="25" spans="1:10" ht="16.2" thickBot="1">
       <c r="A25" s="97">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="103"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="101"/>
+      <c r="C25" s="104">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D25" s="104">
+        <v>0.81458333333333333</v>
+      </c>
+      <c r="E25" s="105">
+        <v>0</v>
+      </c>
+      <c r="F25" s="101">
+        <f t="shared" si="0"/>
+        <v>56.999999999999957</v>
+      </c>
       <c r="G25" s="105" t="s">
         <v>201</v>
       </c>
@@ -8092,7 +8103,7 @@
     </row>
     <row r="26" spans="1:10" ht="16.2" thickBot="1">
       <c r="A26" s="97">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" s="103"/>
       <c r="C26" s="104"/>
@@ -8109,7 +8120,7 @@
     </row>
     <row r="27" spans="1:10" ht="16.2" thickBot="1">
       <c r="A27" s="97">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B27" s="107"/>
       <c r="C27" s="108"/>
@@ -8125,16 +8136,16 @@
       <c r="J27" s="110"/>
     </row>
     <row r="28" spans="1:10" ht="16.2" thickBot="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="144" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="145"/>
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="146"/>
       <c r="F28" s="111">
         <f>SUM(F7:F27)</f>
-        <v>703.99999999999989</v>
+        <v>760.99999999999989</v>
       </c>
       <c r="G28" s="112"/>
       <c r="H28" s="112"/>

</xml_diff>